<commit_message>
fix serious bug parsing date and money
</commit_message>
<xml_diff>
--- a/1_政策宣傳執情形/parsed/農委會/農委會主管102Q1廣宣彙整表.xlsx
+++ b/1_政策宣傳執情形/parsed/農委會/農委會主管102Q1廣宣彙整表.xlsx
@@ -665,7 +665,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
@@ -685,7 +685,7 @@
     <col max="8" min="8" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:8" r="1">
+    <row r="1" spans="1:8">
       <c t="s" r="A1" s="2">
         <v>21</v>
       </c>
@@ -711,7 +711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row spans="1:8" r="2">
+    <row r="2" spans="1:8">
       <c t="s" r="A2">
         <v>44</v>
       </c>
@@ -734,7 +734,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="3">
+    <row r="3" spans="1:8">
       <c t="s" r="A3">
         <v>72</v>
       </c>
@@ -757,7 +757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="4">
+    <row r="4" spans="1:8">
       <c t="s" r="A4">
         <v>72</v>
       </c>
@@ -780,7 +780,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="5">
+    <row r="5" spans="1:8">
       <c t="s" r="A5">
         <v>9</v>
       </c>
@@ -803,7 +803,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="6">
+    <row r="6" spans="1:8">
       <c t="s" r="A6">
         <v>9</v>
       </c>
@@ -826,7 +826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="7">
+    <row r="7" spans="1:8">
       <c t="s" r="A7">
         <v>9</v>
       </c>
@@ -849,7 +849,7 @@
         <v>76</v>
       </c>
     </row>
-    <row spans="1:8" r="8">
+    <row r="8" spans="1:8">
       <c t="s" r="A8">
         <v>9</v>
       </c>
@@ -875,7 +875,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="9">
+    <row r="9" spans="1:8">
       <c t="s" r="A9">
         <v>9</v>
       </c>
@@ -901,7 +901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="10">
+    <row r="10" spans="1:8">
       <c t="s" r="A10">
         <v>71</v>
       </c>
@@ -927,7 +927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="11">
+    <row r="11" spans="1:8">
       <c t="s" r="A11">
         <v>71</v>
       </c>
@@ -953,7 +953,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="12">
+    <row r="12" spans="1:8">
       <c t="s" r="A12">
         <v>71</v>
       </c>
@@ -979,7 +979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="13">
+    <row r="13" spans="1:8">
       <c t="s" r="A13">
         <v>22</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="14">
+    <row r="14" spans="1:8">
       <c t="s" r="A14">
         <v>55</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="15">
+    <row r="15" spans="1:8">
       <c t="s" r="A15">
         <v>55</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="16">
+    <row r="16" spans="1:8">
       <c t="s" r="A16">
         <v>69</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="17">
+    <row r="17" spans="1:8">
       <c t="s" r="A17">
         <v>17</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="18">
+    <row r="18" spans="1:8">
       <c t="s" r="A18">
         <v>80</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="19">
+    <row r="19" spans="1:8">
       <c t="s" r="A19">
         <v>80</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="20">
+    <row r="20" spans="1:8">
       <c t="s" r="A20">
         <v>80</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="21">
+    <row r="21" spans="1:8">
       <c t="s" r="A21">
         <v>56</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="22">
+    <row r="22" spans="1:8">
       <c t="s" r="A22">
         <v>56</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="23">
+    <row r="23" spans="1:8">
       <c t="s" r="A23">
         <v>56</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="24">
+    <row r="24" spans="1:8">
       <c t="s" r="A24">
         <v>56</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="25">
+    <row r="25" spans="1:8">
       <c t="s" r="A25">
         <v>56</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="26">
+    <row r="26" spans="1:8">
       <c t="s" r="A26">
         <v>27</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="27">
+    <row r="27" spans="1:8">
       <c t="s" r="A27">
         <v>27</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="28">
+    <row r="28" spans="1:8">
       <c t="s" r="A28">
         <v>54</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="29">
+    <row r="29" spans="1:8">
       <c t="s" r="A29">
         <v>0</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="30">
+    <row r="30" spans="1:8">
       <c t="s" r="A30">
         <v>59</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="31">
+    <row r="31" spans="1:8">
       <c t="s" r="A31">
         <v>59</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="32">
+    <row r="32" spans="1:8">
       <c t="s" r="A32">
         <v>1</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="33">
+    <row r="33" spans="1:8">
       <c t="s" r="A33">
         <v>1</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="34">
+    <row r="34" spans="1:8">
       <c t="s" r="A34">
         <v>1</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="35">
+    <row r="35" spans="1:8">
       <c t="s" r="A35">
         <v>61</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="36">
+    <row r="36" spans="1:8">
       <c t="s" r="A36">
         <v>62</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="37">
+    <row r="37" spans="1:8">
       <c t="s" r="A37">
         <v>25</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="38">
+    <row r="38" spans="1:8">
       <c t="s" r="A38">
         <v>24</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="39">
+    <row r="39" spans="1:8">
       <c t="s" r="A39">
         <v>43</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="40">
+    <row r="40" spans="1:8">
       <c t="s" r="A40">
         <v>77</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="41">
+    <row r="41" spans="1:8">
       <c t="s" r="A41">
         <v>77</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="42">
+    <row r="42" spans="1:8">
       <c t="s" r="A42">
         <v>77</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="43">
+    <row r="43" spans="1:8">
       <c t="s" r="A43">
         <v>18</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="44">
+    <row r="44" spans="1:8">
       <c t="s" r="A44">
         <v>20</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="45">
+    <row r="45" spans="1:8">
       <c t="s" r="A45">
         <v>19</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>26</v>
       </c>
     </row>
-    <row spans="1:8" r="46">
+    <row r="46" spans="1:8">
       <c t="s" r="A46">
         <v>19</v>
       </c>

</xml_diff>